<commit_message>
Start of 2025 authorlis/membership refresh, make jiscmail and collaboraiton database consistent
</commit_message>
<xml_diff>
--- a/11-CollaborationList/Birmingham.xlsx
+++ b/11-CollaborationList/Birmingham.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/Library/CloudStorage/Box-Box/CubMac-Box/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B61804-90EF-C04E-92C4-BAEF1C14DC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8A2F1722-01CA-584A-B826-747EE5052423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36520" yWindow="1120" windowWidth="28040" windowHeight="17440" xr2:uid="{06771C6B-1973-A943-8791-FC202D4D0B21}"/>
+    <workbookView xWindow="0" yWindow="12120" windowWidth="57600" windowHeight="16220" xr2:uid="{06771C6B-1973-A943-8791-FC202D4D0B21}"/>
   </bookViews>
   <sheets>
     <sheet name="Birmingham" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>Title</t>
   </si>
@@ -127,9 +127,6 @@
     <t>P.</t>
   </si>
   <si>
-    <t>allport@cern.ch</t>
-  </si>
-  <si>
     <t>P. Allport</t>
   </si>
   <si>
@@ -206,13 +203,34 @@
   </si>
   <si>
     <t>E. Melia</t>
+  </si>
+  <si>
+    <t>Tzanka</t>
+  </si>
+  <si>
+    <t>Kokalova-Wheldon</t>
+  </si>
+  <si>
+    <t>t.kokalova@bham.ac.uk; t.wheldon@bham.ac.uk</t>
+  </si>
+  <si>
+    <t>Mx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e.melia.1@bham.ac.uk </t>
+  </si>
+  <si>
+    <t>E.Melia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allport@cern.ch; philip.patrick.allport@cern.ch </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -347,6 +365,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -529,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -644,8 +670,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -688,11 +725,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -726,6 +766,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1090,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C17739-54D2-4D47-931C-4023B7093A8F}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1102,7 +1143,7 @@
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="117.33203125" bestFit="1" customWidth="1"/>
@@ -1185,7 +1226,7 @@
         <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1243,22 +1284,22 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O4" t="s">
         <v>22</v>
@@ -1266,28 +1307,28 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
       <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1298,28 +1339,28 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
       <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1327,28 +1368,28 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
         <v>53</v>
       </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>54</v>
       </c>
-      <c r="F7" t="s">
-        <v>55</v>
-      </c>
       <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
         <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1356,22 +1397,22 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
         <v>57</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>58</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>59</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>60</v>
-      </c>
-      <c r="F8" t="s">
-        <v>61</v>
       </c>
       <c r="G8" t="s">
         <v>28</v>
@@ -1383,10 +1424,72 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E9" r:id="rId1" display="t.kokalova@bham.ac.uk;t.wheldon@bham.ac.uk" xr:uid="{18ECC978-62F8-994C-B266-AC2888889F7E}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{48B28EA3-3E52-9141-837C-5F79D3C98AD6}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to make draft version for circulation
</commit_message>
<xml_diff>
--- a/11-CollaborationList/Birmingham.xlsx
+++ b/11-CollaborationList/Birmingham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2050112264517/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{18CD952A-1DAB-DF47-86C4-62F9FCF0F0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AAC35B4-790D-7140-A5EA-1307193559C2}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{18CD952A-1DAB-DF47-86C4-62F9FCF0F0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{505C5F60-4C0C-4948-97B4-51682916384F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{06771C6B-1973-A943-8791-FC202D4D0B21}"/>
   </bookViews>
@@ -154,10 +154,10 @@
     <t>E.Melia</t>
   </si>
   <si>
-    <t>e.melia.1@bham.ac.uk; exm307@student.bham.ac.uk</t>
-  </si>
-  <si>
     <t>Dr.</t>
+  </si>
+  <si>
+    <t>e.melia.1@bham.ac.uk</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1068,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -1250,7 +1250,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
         <v>43</v>
@@ -1267,7 +1267,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" display="e.melia.1@bham.ac.uk " xr:uid="{48B28EA3-3E52-9141-837C-5F79D3C98AD6}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{48B28EA3-3E52-9141-837C-5F79D3C98AD6}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>